<commit_message>
Create function to add information from excel to database.
</commit_message>
<xml_diff>
--- a/professional experiences.xlsx
+++ b/professional experiences.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\Web development\MyResume\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997DE2D5-BB15-4F2D-BF3A-BC9052DB0182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75AE3281-E582-49BA-9D47-2F928EEC32AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-10830" windowWidth="16440" windowHeight="28440" xr2:uid="{69BFDC15-D326-45E4-BC27-3FC6D42695F1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{69BFDC15-D326-45E4-BC27-3FC6D42695F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
   <si>
     <t>Stanley Black &amp; Decker. Medellín, Colombia.</t>
   </si>
@@ -183,6 +183,24 @@
   </si>
   <si>
     <t>Strategic Planning Collector</t>
+  </si>
+  <si>
+    <t>../static/images/Certifications/Certificate-Python-Bootcamp.png</t>
+  </si>
+  <si>
+    <t>../static/images/Certifications/Certificate-Python-Django-Bootcamp.png</t>
+  </si>
+  <si>
+    <t>../static/images/Certifications/PR Certification.png</t>
+  </si>
+  <si>
+    <t>../static/images/Certifications/SEO Certification.png</t>
+  </si>
+  <si>
+    <t>img</t>
+  </si>
+  <si>
+    <t>cert</t>
   </si>
 </sst>
 </file>
@@ -536,7 +554,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C11F4FC-4BEB-4BB8-890C-62E074A1B1EC}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -727,29 +745,59 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17285960-922A-4935-8077-76BC31C8AA69}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
         <v>43</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
         <v>44</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
         <v>45</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
         <v>46</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add recaptcha form to message
</commit_message>
<xml_diff>
--- a/professional experiences.xlsx
+++ b/professional experiences.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\Web development\MyResume\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B55D64A-DF19-486B-8FF5-E0F3F089F628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF1AE35-7720-42BA-B2A6-D1F86860C67E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{69BFDC15-D326-45E4-BC27-3FC6D42695F1}"/>
   </bookViews>
@@ -128,9 +128,6 @@
     <t>Freelance Upwork</t>
   </si>
   <si>
-    <t>December 2021 - Present</t>
-  </si>
-  <si>
     <t>https://udemy-certificate.s3.amazonaws.com/image/UC-b527ed3c-4fd0-4701-bc19-09d06acf6bfe.jpg</t>
   </si>
   <si>
@@ -201,6 +198,9 @@
   </si>
   <si>
     <t>Keyword Research.</t>
+  </si>
+  <si>
+    <t>December 2021 - April 2022</t>
   </si>
 </sst>
 </file>
@@ -555,7 +555,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,10 +588,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
         <v>35</v>
-      </c>
-      <c r="B2" t="s">
-        <v>36</v>
       </c>
       <c r="C2" t="s">
         <v>26</v>
@@ -608,10 +608,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -628,10 +628,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -648,10 +648,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -665,10 +665,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -682,7 +682,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
         <v>28</v>
@@ -696,7 +696,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
@@ -707,7 +707,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -715,7 +715,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C10" t="s">
         <v>12</v>
@@ -723,7 +723,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="C11" t="s">
         <v>13</v>
@@ -760,42 +760,42 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
         <v>41</v>
-      </c>
-      <c r="B1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix order of certificates
</commit_message>
<xml_diff>
--- a/professional experiences.xlsx
+++ b/professional experiences.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\Web development\MyResume\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87A13EC-0D7B-43A6-9D0F-68E6A293F881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B7ED3CB-42C8-4866-A4CE-1C9D5CAAF574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-12885" windowWidth="16440" windowHeight="28440" activeTab="1" xr2:uid="{69BFDC15-D326-45E4-BC27-3FC6D42695F1}"/>
   </bookViews>
@@ -802,42 +802,42 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix url for image cert
</commit_message>
<xml_diff>
--- a/professional experiences.xlsx
+++ b/professional experiences.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\Web development\MyResume\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B7ED3CB-42C8-4866-A4CE-1C9D5CAAF574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85CD3031-6808-4AA7-9F1E-E817BCA6AFFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-12885" windowWidth="16440" windowHeight="28440" activeTab="1" xr2:uid="{69BFDC15-D326-45E4-BC27-3FC6D42695F1}"/>
   </bookViews>
@@ -218,7 +218,7 @@
     <t>https://udemy-certificate.s3.amazonaws.com/image/UC-4394f62e-a654-491d-9e22-d09c11d6d9aa.jpg</t>
   </si>
   <si>
-    <t>../static/images/Certifications/AdvSQL.png</t>
+    <t>../static/images/Certifications/Certificate-AdvSQL.png</t>
   </si>
 </sst>
 </file>
@@ -768,7 +768,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>